<commit_message>
Revised the offset operation for activation results.
</commit_message>
<xml_diff>
--- a/Assignment01/workplace(genre)/Results.xlsx
+++ b/Assignment01/workplace(genre)/Results.xlsx
@@ -19,13 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Indexing</t>
-  </si>
-  <si>
-    <t>Pruning strategies</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Accuracy</t>
   </si>
@@ -39,40 +33,7 @@
     <t>F1 Score</t>
   </si>
   <si>
-    <t>(No pruning)</t>
-  </si>
-  <si>
-    <t>(I)</t>
-  </si>
-  <si>
-    <t>(3  -&gt; 18)</t>
-  </si>
-  <si>
-    <t>(II)</t>
-  </si>
-  <si>
-    <t>(29 -&gt; 25)</t>
-  </si>
-  <si>
-    <t>(III)</t>
-  </si>
-  <si>
-    <t>(25 -&gt; 29) (16 -&gt; 2)</t>
-  </si>
-  <si>
-    <t>(IV)</t>
-  </si>
-  <si>
-    <t>(25 -&gt; 29) (16 -&gt; 2) (3  -&gt; 18)</t>
-  </si>
-  <si>
-    <t>(V)</t>
-  </si>
-  <si>
-    <t>(25 -&gt; 29) (16 -&gt; 2) (17 -&gt; 1)</t>
-  </si>
-  <si>
-    <t>(VI)</t>
+    <t>hidden units</t>
   </si>
 </sst>
 </file>
@@ -102,27 +63,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -133,19 +79,6 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top/>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -166,18 +99,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -231,14 +161,16 @@
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN"/>
-              <a:t>Classification Based</a:t>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1" baseline="0"/>
+              <a:t>NN Classification Based on </a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
-              <a:t> on Music Genre</a:t>
+              <a:rPr lang="en-US" sz="1600" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Electric Signals </a:t>
             </a:r>
-            <a:endParaRPr lang="zh-CN" altLang="en-US"/>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1600" b="1"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -284,14 +216,11 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$2:$B$2</c:f>
+              <c:f>Sheet1!$A$2:$A$2</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>(I)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>(No pruning)</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -308,7 +237,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$1:$F$1</c:f>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -328,21 +257,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$F$2</c:f>
+              <c:f>Sheet1!$B$2:$E$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.64710000000000001</c:v>
+                  <c:v>0.63749999999999996</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.37219999999999998</c:v>
+                  <c:v>0.62809999999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.52780000000000005</c:v>
+                  <c:v>0.6653</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.40379999999999999</c:v>
+                  <c:v>0.6431</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -358,14 +287,11 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$3:$B$3</c:f>
+              <c:f>Sheet1!$A$3:$A$3</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>(II)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>(3  -&gt; 18)</c:v>
+                  <c:v>29</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -382,7 +308,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$1:$F$1</c:f>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -402,21 +328,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$3:$F$3</c:f>
+              <c:f>Sheet1!$B$3:$E$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.61760000000000004</c:v>
+                  <c:v>0.69579999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.35089999999999999</c:v>
+                  <c:v>0.63439999999999996</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.50929999999999997</c:v>
+                  <c:v>0.64539999999999997</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.38</c:v>
+                  <c:v>0.59970000000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -432,14 +358,11 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$4:$B$4</c:f>
+              <c:f>Sheet1!$A$4:$A$4</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>(III)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>(29 -&gt; 25)</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -456,7 +379,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$1:$F$1</c:f>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -476,21 +399,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$F$4</c:f>
+              <c:f>Sheet1!$B$4:$E$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.64710000000000001</c:v>
+                  <c:v>0.67510000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.37219999999999998</c:v>
+                  <c:v>0.5222</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.52780000000000005</c:v>
+                  <c:v>0.63929999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.40379999999999999</c:v>
+                  <c:v>0.52759999999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -506,14 +429,11 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$5:$B$5</c:f>
+              <c:f>Sheet1!$A$5:$A$5</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>(IV)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>(25 -&gt; 29) (16 -&gt; 2)</c:v>
+                  <c:v>27</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -530,7 +450,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$1:$F$1</c:f>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -550,21 +470,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$5:$F$5</c:f>
+              <c:f>Sheet1!$B$5:$E$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.61760000000000004</c:v>
+                  <c:v>0.61250000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43940000000000001</c:v>
+                  <c:v>0.74439999999999995</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.50929999999999997</c:v>
+                  <c:v>0.6321</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.3866</c:v>
+                  <c:v>0.50109999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -580,14 +500,11 @@
           <c:order val="4"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$A$6:$B$6</c:f>
+              <c:f>Sheet1!$A$6:$A$6</c:f>
               <c:strCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>(V)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>(25 -&gt; 29) (16 -&gt; 2) (3  -&gt; 18)</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -604,7 +521,7 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>Sheet1!$C$1:$F$1</c:f>
+              <c:f>Sheet1!$B$1:$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
@@ -624,21 +541,21 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$6:$F$6</c:f>
+              <c:f>Sheet1!$B$6:$E$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.52939999999999998</c:v>
+                  <c:v>0.55249999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.2576</c:v>
+                  <c:v>0.73850000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.45</c:v>
+                  <c:v>0.62150000000000005</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.32500000000000001</c:v>
+                  <c:v>0.58220000000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -649,81 +566,8 @@
             </c:ext>
           </c:extLst>
         </c:ser>
-        <c:ser>
-          <c:idx val="5"/>
-          <c:order val="5"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet1!$A$7:$B$7</c:f>
-              <c:strCache>
-                <c:ptCount val="2"/>
-                <c:pt idx="0">
-                  <c:v>(VI)</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>(25 -&gt; 29) (16 -&gt; 2) (17 -&gt; 1)</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent6"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet1!$C$1:$F$1</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>Accuracy</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>Precision</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>Recall</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>F1 Score</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet1!$C$7:$F$7</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>0.64710000000000001</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.30980000000000002</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.43059999999999998</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.31719999999999998</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-441B-42B6-BF5D-A11DBF0A52D1}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
+          <c:dLblPos val="outEnd"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -966,15 +810,15 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="r"/>
       <c:layout>
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="9.1660138464834756E-2"/>
-          <c:y val="0.10672845863371097"/>
-          <c:w val="0.79542121966896995"/>
-          <c:h val="0.11071141853921193"/>
+          <c:x val="0.92886094687990994"/>
+          <c:y val="0.36872597006455277"/>
+          <c:w val="7.1139053120090098E-2"/>
+          <c:h val="0.38007022770802296"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1006,6 +850,543 @@
         </a:p>
       </c:txPr>
     </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1"/>
+              <a:t>NN Test Computation Time Based on Electric</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" altLang="zh-CN" sz="1600" b="1" baseline="0"/>
+              <a:t> Signals</a:t>
+            </a:r>
+            <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1600" b="1"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="75000"/>
+                        <a:lumOff val="25000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="t"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="35000"/>
+                          <a:lumOff val="65000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:round/>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$A$2:$A$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>26</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$G$2:$G$7</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>2.500607</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2998189999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7015610000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.4998910000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.6982219999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.483644</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3A22-4847-9ADD-A465876C329C}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="t"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1750334511"/>
+        <c:axId val="1750327023"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1750334511"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1"/>
+                  <a:t>Number of Hidden Units</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1750327023"/>
+        <c:crossesAt val="1.4"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1750327023"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="1.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:rPr>
+                  <a:t>Time</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" sz="1400" b="1"/>
+                  <a:t> (ms)</a:t>
+                </a:r>
+                <a:endParaRPr lang="zh-CN" altLang="en-US" sz="1400" b="1"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1750334511"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="0.2"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -1083,6 +1464,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -1586,20 +2007,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>137160</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>457200</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1613,6 +2550,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>312420</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>11430</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="图表 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1884,160 +2851,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="11.88671875" customWidth="1"/>
+    <col min="3" max="3" width="12.5546875" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0.64710000000000001</v>
-      </c>
-      <c r="D2" s="4">
-        <v>0.37219999999999998</v>
-      </c>
-      <c r="E2" s="4">
-        <v>0.52780000000000005</v>
-      </c>
-      <c r="F2" s="4">
-        <v>0.40379999999999999</v>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="2">
+        <v>30</v>
+      </c>
+      <c r="B2" s="2">
+        <v>0.63749999999999996</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.62809999999999999</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.6653</v>
+      </c>
+      <c r="E2" s="2">
+        <v>0.6431</v>
+      </c>
+      <c r="G2" s="3">
+        <v>2.500607</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0.61760000000000004</v>
-      </c>
-      <c r="D3" s="4">
-        <v>0.35089999999999999</v>
-      </c>
-      <c r="E3" s="4">
-        <v>0.50929999999999997</v>
-      </c>
-      <c r="F3" s="4">
-        <v>0.38</v>
+    <row r="3" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2">
+        <v>0.69579999999999997</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.63439999999999996</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.64539999999999997</v>
+      </c>
+      <c r="E3" s="2">
+        <v>0.59970000000000001</v>
+      </c>
+      <c r="G3" s="3">
+        <v>2.2998189999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0.64710000000000001</v>
-      </c>
-      <c r="D4" s="4">
-        <v>0.37219999999999998</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0.52780000000000005</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0.40379999999999999</v>
+    <row r="4" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="2">
+        <v>28</v>
+      </c>
+      <c r="B4" s="2">
+        <v>0.67510000000000003</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.5222</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.63929999999999998</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0.52759999999999996</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1.7015610000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="4">
-        <v>0.61760000000000004</v>
-      </c>
-      <c r="D5" s="4">
-        <v>0.43940000000000001</v>
-      </c>
-      <c r="E5" s="4">
-        <v>0.50929999999999997</v>
-      </c>
-      <c r="F5" s="4">
-        <v>0.3866</v>
+    <row r="5" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="2">
+        <v>27</v>
+      </c>
+      <c r="B5" s="2">
+        <v>0.61250000000000004</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.74439999999999995</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.6321</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.50109999999999999</v>
+      </c>
+      <c r="G5" s="3">
+        <v>1.4998910000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="4">
-        <v>0.52939999999999998</v>
-      </c>
-      <c r="D6" s="4">
-        <v>0.2576</v>
-      </c>
-      <c r="E6" s="4">
-        <v>0.45</v>
-      </c>
-      <c r="F6" s="4">
-        <v>0.32500000000000001</v>
+    <row r="6" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2">
+        <v>26</v>
+      </c>
+      <c r="B6" s="2">
+        <v>0.55249999999999999</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.73850000000000005</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.62150000000000005</v>
+      </c>
+      <c r="E6" s="2">
+        <v>0.58220000000000005</v>
+      </c>
+      <c r="G6" s="3">
+        <v>1.6982219999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" s="4">
-        <v>0.64710000000000001</v>
-      </c>
-      <c r="D7" s="4">
-        <v>0.30980000000000002</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.43059999999999998</v>
-      </c>
-      <c r="F7" s="4">
-        <v>0.31719999999999998</v>
+    <row r="7" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2">
+        <v>26</v>
+      </c>
+      <c r="B7" s="2">
+        <v>0.51749999999999996</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.6714</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.61539999999999995</v>
+      </c>
+      <c r="E7" s="2">
+        <v>0.53439999999999999</v>
+      </c>
+      <c r="G7" s="3">
+        <v>1.483644</v>
       </c>
     </row>
   </sheetData>

</xml_diff>